<commit_message>
DSS - VerDespesasPorPagar e VerDespesasPagas
</commit_message>
<xml_diff>
--- a/Fase 2/F2-Descrição_use_cases.xlsx
+++ b/Fase 2/F2-Descrição_use_cases.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="17426"/>
+  <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\João\Documents\GitHub\dss-1617\Fase 2\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\UM\Informática\3º Ano\1º Semestre\DSS\dss-1617\Fase 2\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="450" windowWidth="23040" windowHeight="8805" tabRatio="856" firstSheet="5" activeTab="7"/>
+    <workbookView xWindow="0" yWindow="450" windowWidth="23040" windowHeight="8808" tabRatio="856" firstSheet="4" activeTab="8"/>
   </bookViews>
   <sheets>
     <sheet name="Regista Apartamento" sheetId="7" r:id="rId1"/>
@@ -25,7 +25,7 @@
     <sheet name="Pagar Despesa" sheetId="10" r:id="rId11"/>
     <sheet name="Carregar Conta" sheetId="5" r:id="rId12"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="171027"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="237" uniqueCount="110">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="244" uniqueCount="114">
   <si>
     <r>
       <t xml:space="preserve">  </t>
@@ -365,13 +365,6 @@
     <t>Indica que o apartamento foi registado</t>
   </si>
   <si>
-    <t>Excepção 1               (passo 2)
-[apartamento já existe no sistema]</t>
-  </si>
-  <si>
-    <t>Indica que o apartamento já existe</t>
-  </si>
-  <si>
     <t>Fornece dados do apartamento</t>
   </si>
   <si>
@@ -385,15 +378,6 @@
   </si>
   <si>
     <t>Atualiza fração da renda dos restantes moradores, caso existam</t>
-  </si>
-  <si>
-    <t>Seleciona o(s) morador(es)</t>
-  </si>
-  <si>
-    <t>Apresenta a lista das despesas do(s) morador(es)</t>
-  </si>
-  <si>
-    <t>Apresenta a lista das despesas pagas pelo(s) morador(es)</t>
   </si>
   <si>
     <t>Acrescenta o valor ao saldo da conta</t>
@@ -425,12 +409,41 @@
   </si>
   <si>
     <t>Altera renda do apartamento</t>
+  </si>
+  <si>
+    <t>Indica que quer ver despesas por pagar</t>
+  </si>
+  <si>
+    <t>Seleciona o morador</t>
+  </si>
+  <si>
+    <t>Apresenta a lista das despesas do morador</t>
+  </si>
+  <si>
+    <t>Indica que já existe um apartamento no sistema</t>
+  </si>
+  <si>
+    <t>Verifica se existe um apartamento</t>
+  </si>
+  <si>
+    <t>Excepção 1               (passo 1)
+[já existe um apartamento no sistema]</t>
+  </si>
+  <si>
+    <t>Excepção 2               (passo 3)
+[dados do apartamento inválidos]</t>
+  </si>
+  <si>
+    <t>Indica que quer ver despesas pagas</t>
+  </si>
+  <si>
+    <t>Apresenta a lista das despesas pagas pelo morador</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -491,7 +504,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -524,6 +537,9 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -839,22 +855,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A3:D14"/>
+  <dimension ref="A3:D19"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="A10" sqref="A10:D17"/>
+      <selection activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.83984375" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col min="1" max="1" width="15.140625" style="5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8.85546875" style="5"/>
-    <col min="3" max="3" width="30.140625" style="5" customWidth="1"/>
-    <col min="4" max="4" width="32.7109375" style="5" customWidth="1"/>
-    <col min="5" max="16384" width="8.85546875" style="1"/>
+    <col min="1" max="1" width="15.15625" style="5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.83984375" style="5"/>
+    <col min="3" max="3" width="30.15625" style="5" customWidth="1"/>
+    <col min="4" max="4" width="32.68359375" style="5" customWidth="1"/>
+    <col min="5" max="16384" width="8.83984375" style="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" s="4" t="s">
         <v>6</v>
       </c>
@@ -862,7 +878,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" s="5" t="s">
         <v>0</v>
       </c>
@@ -870,17 +886,17 @@
         <v>53</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" s="5" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" s="5" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="C7" s="4" t="s">
         <v>4</v>
       </c>
@@ -888,68 +904,108 @@
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A8" s="5" t="s">
         <v>3</v>
       </c>
       <c r="B8" s="5">
         <v>1</v>
       </c>
-      <c r="C8" s="5" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C8" s="1"/>
+      <c r="D8" s="5" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="B9" s="5">
-        <v>2</v>
-      </c>
-      <c r="D9" s="5" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+        <f>B8+1</f>
+        <v>2</v>
+      </c>
+      <c r="C9" s="5" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="B10" s="5">
+        <f t="shared" ref="B10:B12" si="0">B9+1</f>
         <v>3</v>
       </c>
       <c r="D10" s="5" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="B11" s="5">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="D11" s="5" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B11" s="5">
-        <v>4</v>
-      </c>
-      <c r="D11" s="5" t="s">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="B12" s="5">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="D12" s="5" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A12" s="8"/>
-      <c r="B12" s="4"/>
-      <c r="C12" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="D12" s="4" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" ht="75" x14ac:dyDescent="0.25">
-      <c r="A13" s="7" t="s">
-        <v>90</v>
-      </c>
-      <c r="B13" s="5">
-        <v>1</v>
-      </c>
-      <c r="D13" s="5" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A14" s="7"/>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A13" s="8"/>
+      <c r="B13" s="4"/>
+      <c r="C13" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="D13" s="4" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" ht="72" x14ac:dyDescent="0.55000000000000004">
+      <c r="A14" s="7" t="s">
+        <v>110</v>
+      </c>
       <c r="B14" s="5">
-        <v>2</v>
-      </c>
-      <c r="D14" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="D14" s="13" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A15" s="7"/>
+      <c r="B15" s="5">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A17" s="8"/>
+      <c r="B17" s="4"/>
+      <c r="C17" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="D17" s="4" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" ht="72" x14ac:dyDescent="0.55000000000000004">
+      <c r="A18" s="7" t="s">
+        <v>111</v>
+      </c>
+      <c r="B18" s="5">
+        <v>1</v>
+      </c>
+      <c r="D18" s="13" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A19" s="7"/>
+      <c r="B19" s="5">
+        <v>2</v>
+      </c>
+      <c r="D19" s="5" t="s">
         <v>18</v>
       </c>
     </row>
@@ -967,16 +1023,16 @@
       <selection activeCell="G18" sqref="G18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.83984375" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col min="1" max="1" width="15.140625" style="5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8.85546875" style="5"/>
-    <col min="3" max="3" width="34.85546875" style="5" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="15.15625" style="5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.83984375" style="5"/>
+    <col min="3" max="3" width="34.83984375" style="5" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="40" style="5" bestFit="1" customWidth="1"/>
-    <col min="5" max="16384" width="8.85546875" style="1"/>
+    <col min="5" max="16384" width="8.83984375" style="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" s="4" t="s">
         <v>6</v>
       </c>
@@ -984,7 +1040,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" s="5" t="s">
         <v>0</v>
       </c>
@@ -992,17 +1048,17 @@
         <v>65</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" s="5" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" s="5" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="C7" s="4" t="s">
         <v>4</v>
       </c>
@@ -1010,7 +1066,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A8" s="5" t="s">
         <v>3</v>
       </c>
@@ -1021,7 +1077,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="B9" s="5">
         <v>2</v>
       </c>
@@ -1029,7 +1085,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="B10" s="5">
         <v>3</v>
       </c>
@@ -1037,10 +1093,10 @@
         <v>68</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A11" s="6"/>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A12" s="6"/>
       <c r="C12" s="4" t="s">
         <v>4</v>
@@ -1049,7 +1105,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="13" spans="1:4" ht="75" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4" ht="72" x14ac:dyDescent="0.55000000000000004">
       <c r="A13" s="7" t="s">
         <v>69</v>
       </c>
@@ -1060,7 +1116,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="B14" s="5">
         <v>2</v>
       </c>
@@ -1082,16 +1138,16 @@
       <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.83984375" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col min="1" max="1" width="15.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8.85546875" style="1"/>
-    <col min="3" max="3" width="48.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="53.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="16384" width="8.85546875" style="1"/>
+    <col min="1" max="1" width="15.15625" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.83984375" style="1"/>
+    <col min="3" max="3" width="48.41796875" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="53.578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="16384" width="8.83984375" style="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" s="3" t="s">
         <v>6</v>
       </c>
@@ -1099,7 +1155,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" s="1" t="s">
         <v>0</v>
       </c>
@@ -1107,7 +1163,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" s="1" t="s">
         <v>1</v>
       </c>
@@ -1115,12 +1171,12 @@
         <v>73</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" s="1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="C7" s="3" t="s">
         <v>4</v>
       </c>
@@ -1128,7 +1184,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A8" s="1" t="s">
         <v>3</v>
       </c>
@@ -1136,11 +1192,11 @@
         <v>1</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>101</v>
+        <v>96</v>
       </c>
       <c r="K8" s="10"/>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="B9" s="1">
         <f>B8+1</f>
         <v>2</v>
@@ -1149,7 +1205,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A10"/>
       <c r="B10" s="1">
         <f t="shared" ref="B10:B16" si="0">B9+1</f>
@@ -1160,7 +1216,7 @@
       </c>
       <c r="D10" s="10"/>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A11"/>
       <c r="B11" s="1">
         <f t="shared" si="0"/>
@@ -1170,7 +1226,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A12"/>
       <c r="B12" s="1">
         <f t="shared" si="0"/>
@@ -1180,7 +1236,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A13"/>
       <c r="B13" s="1">
         <f t="shared" si="0"/>
@@ -1190,7 +1246,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A14"/>
       <c r="B14" s="1">
         <f t="shared" si="0"/>
@@ -1200,7 +1256,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A15"/>
       <c r="B15" s="1">
         <f t="shared" si="0"/>
@@ -1210,7 +1266,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A16"/>
       <c r="B16" s="1">
         <f t="shared" si="0"/>
@@ -1220,7 +1276,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A17"/>
       <c r="C17" s="3" t="s">
         <v>4</v>
@@ -1229,9 +1285,9 @@
         <v>5</v>
       </c>
     </row>
-    <row r="18" spans="1:4" ht="60" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:4" ht="57.6" x14ac:dyDescent="0.55000000000000004">
       <c r="A18" s="2" t="s">
-        <v>102</v>
+        <v>97</v>
       </c>
       <c r="B18" s="1">
         <v>1</v>
@@ -1254,16 +1310,16 @@
       <selection activeCell="H10" sqref="H10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.83984375" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col min="1" max="1" width="15.140625" style="5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8.85546875" style="5"/>
-    <col min="3" max="3" width="35.42578125" style="5" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="32.7109375" style="5" customWidth="1"/>
-    <col min="5" max="16384" width="8.85546875" style="1"/>
+    <col min="1" max="1" width="15.15625" style="5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.83984375" style="5"/>
+    <col min="3" max="3" width="35.41796875" style="5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="32.68359375" style="5" customWidth="1"/>
+    <col min="5" max="16384" width="8.83984375" style="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" s="4" t="s">
         <v>6</v>
       </c>
@@ -1271,7 +1327,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" s="5" t="s">
         <v>0</v>
       </c>
@@ -1279,7 +1335,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" s="5" t="s">
         <v>1</v>
       </c>
@@ -1287,12 +1343,12 @@
         <v>85</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" s="5" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="C7" s="4" t="s">
         <v>4</v>
       </c>
@@ -1300,7 +1356,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A8" s="5" t="s">
         <v>3</v>
       </c>
@@ -1308,10 +1364,10 @@
         <v>1</v>
       </c>
       <c r="D8" s="5" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="B9" s="5">
         <v>2</v>
       </c>
@@ -1319,15 +1375,15 @@
         <v>86</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="B10" s="5">
         <v>3</v>
       </c>
       <c r="D10" s="5" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A11" s="6"/>
       <c r="B11" s="5">
         <v>4</v>
@@ -1336,7 +1392,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A12" s="6"/>
       <c r="B12" s="5">
         <v>5</v>
@@ -1345,15 +1401,15 @@
         <v>88</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A13" s="6"/>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A14" s="6"/>
       <c r="C14" s="4"/>
       <c r="D14" s="4"/>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A15" s="7"/>
     </row>
   </sheetData>
@@ -1370,16 +1426,16 @@
       <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.83984375" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col min="1" max="1" width="20.140625" style="5" customWidth="1"/>
-    <col min="2" max="2" width="8.85546875" style="5"/>
-    <col min="3" max="3" width="46.7109375" style="5" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="51.28515625" style="5" bestFit="1" customWidth="1"/>
-    <col min="5" max="16384" width="8.85546875" style="1"/>
+    <col min="1" max="1" width="20.15625" style="5" customWidth="1"/>
+    <col min="2" max="2" width="8.83984375" style="5"/>
+    <col min="3" max="3" width="46.68359375" style="5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="51.26171875" style="5" bestFit="1" customWidth="1"/>
+    <col min="5" max="16384" width="8.83984375" style="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" s="4" t="s">
         <v>6</v>
       </c>
@@ -1387,7 +1443,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" s="5" t="s">
         <v>0</v>
       </c>
@@ -1395,7 +1451,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" s="5" t="s">
         <v>1</v>
       </c>
@@ -1403,7 +1459,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" s="5" t="s">
         <v>2</v>
       </c>
@@ -1411,7 +1467,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="7" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A7" s="4"/>
       <c r="B7" s="4"/>
       <c r="C7" s="4" t="s">
@@ -1421,7 +1477,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A8" s="4" t="s">
         <v>20</v>
       </c>
@@ -1433,23 +1489,23 @@
       </c>
       <c r="D8" s="4"/>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="B9" s="5">
         <v>2</v>
       </c>
       <c r="D9" s="5" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="B10" s="5">
         <v>3</v>
       </c>
       <c r="D10" s="5" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A11" s="6"/>
       <c r="B11" s="5">
         <v>4</v>
@@ -1459,7 +1515,7 @@
       </c>
       <c r="F11" s="10"/>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="B12" s="5">
         <v>5</v>
       </c>
@@ -1467,15 +1523,15 @@
         <v>12</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="B13" s="5">
         <v>6</v>
       </c>
       <c r="C13" s="5" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="B14" s="5">
         <v>7</v>
       </c>
@@ -1483,15 +1539,15 @@
         <v>55</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="B15" s="5">
         <v>8</v>
       </c>
       <c r="D15" s="5" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="B16" s="5">
         <v>9</v>
       </c>
@@ -1499,7 +1555,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A17" s="8"/>
       <c r="B17" s="4"/>
       <c r="C17" s="4" t="s">
@@ -1509,7 +1565,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="18" spans="1:4" s="3" customFormat="1" ht="60" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:4" s="3" customFormat="1" ht="57.6" x14ac:dyDescent="0.55000000000000004">
       <c r="A18" s="7" t="s">
         <v>14</v>
       </c>
@@ -1521,7 +1577,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="B19" s="5">
         <v>2</v>
       </c>
@@ -1529,7 +1585,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A20" s="8"/>
       <c r="B20" s="4"/>
       <c r="C20" s="4" t="s">
@@ -1539,7 +1595,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="21" spans="1:4" s="3" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:4" s="3" customFormat="1" ht="43.2" x14ac:dyDescent="0.55000000000000004">
       <c r="A21" s="7" t="s">
         <v>16</v>
       </c>
@@ -1551,7 +1607,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="B22" s="5">
         <v>2</v>
       </c>
@@ -1559,22 +1615,22 @@
         <v>18</v>
       </c>
     </row>
-    <row r="25" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A25" s="8"/>
       <c r="B25" s="4"/>
       <c r="C25" s="4"/>
       <c r="D25" s="4"/>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A26" s="7"/>
     </row>
-    <row r="33" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A33" s="8"/>
       <c r="B33" s="4"/>
       <c r="C33" s="4"/>
       <c r="D33" s="4"/>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A34" s="7"/>
     </row>
   </sheetData>
@@ -1591,16 +1647,16 @@
       <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.83984375" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col min="1" max="1" width="15.140625" style="5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8.85546875" style="5"/>
+    <col min="1" max="1" width="15.15625" style="5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.83984375" style="5"/>
     <col min="3" max="3" width="48" style="5" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="43.85546875" style="5" bestFit="1" customWidth="1"/>
-    <col min="5" max="16384" width="8.85546875" style="1"/>
+    <col min="4" max="4" width="43.83984375" style="5" bestFit="1" customWidth="1"/>
+    <col min="5" max="16384" width="8.83984375" style="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" s="4" t="s">
         <v>6</v>
       </c>
@@ -1608,7 +1664,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" s="5" t="s">
         <v>0</v>
       </c>
@@ -1616,7 +1672,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" s="5" t="s">
         <v>1</v>
       </c>
@@ -1624,7 +1680,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" s="5" t="s">
         <v>2</v>
       </c>
@@ -1633,7 +1689,7 @@
       </c>
       <c r="G6" s="5"/>
     </row>
-    <row r="7" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A7" s="4"/>
       <c r="B7" s="4"/>
       <c r="C7" s="4" t="s">
@@ -1643,7 +1699,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A8" s="5" t="s">
         <v>3</v>
       </c>
@@ -1654,7 +1710,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="B9" s="5">
         <v>2</v>
       </c>
@@ -1662,7 +1718,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="B10" s="5">
         <v>3</v>
       </c>
@@ -1670,7 +1726,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="B11" s="5">
         <v>4</v>
       </c>
@@ -1679,7 +1735,7 @@
       </c>
       <c r="H11" s="10"/>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="B12" s="5">
         <v>5</v>
       </c>
@@ -1687,7 +1743,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="B13" s="5">
         <v>7</v>
       </c>
@@ -1695,7 +1751,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A14" s="8"/>
       <c r="B14" s="4"/>
       <c r="C14" s="4" t="s">
@@ -1705,7 +1761,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="15" spans="1:10" s="3" customFormat="1" ht="75" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:10" s="3" customFormat="1" ht="72" x14ac:dyDescent="0.55000000000000004">
       <c r="A15" s="7" t="s">
         <v>25</v>
       </c>
@@ -1717,7 +1773,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A16" s="6"/>
       <c r="B16" s="5">
         <v>2</v>
@@ -1727,7 +1783,7 @@
       </c>
       <c r="J16" s="10"/>
     </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:1" x14ac:dyDescent="0.55000000000000004">
       <c r="A18" s="7"/>
     </row>
   </sheetData>
@@ -1744,16 +1800,16 @@
       <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.83984375" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col min="1" max="1" width="15.140625" style="5" customWidth="1"/>
-    <col min="2" max="2" width="8.85546875" style="5"/>
-    <col min="3" max="3" width="44.28515625" style="5" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="39.5703125" style="5" bestFit="1" customWidth="1"/>
-    <col min="5" max="16384" width="8.85546875" style="1"/>
+    <col min="1" max="1" width="15.15625" style="5" customWidth="1"/>
+    <col min="2" max="2" width="8.83984375" style="5"/>
+    <col min="3" max="3" width="44.26171875" style="5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="39.578125" style="5" bestFit="1" customWidth="1"/>
+    <col min="5" max="16384" width="8.83984375" style="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" s="4" t="s">
         <v>6</v>
       </c>
@@ -1761,7 +1817,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" s="5" t="s">
         <v>0</v>
       </c>
@@ -1769,7 +1825,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" s="5" t="s">
         <v>1</v>
       </c>
@@ -1777,12 +1833,12 @@
         <v>32</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" s="5" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A7" s="4"/>
       <c r="B7" s="4"/>
       <c r="C7" s="4" t="s">
@@ -1792,7 +1848,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A8" s="5" t="s">
         <v>3</v>
       </c>
@@ -1803,7 +1859,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="B9" s="5">
         <v>2</v>
       </c>
@@ -1811,7 +1867,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="B10" s="5">
         <v>3</v>
       </c>
@@ -1819,7 +1875,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="B11" s="5">
         <v>4</v>
       </c>
@@ -1827,7 +1883,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="B12" s="5">
         <v>5</v>
       </c>
@@ -1835,7 +1891,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="B13" s="5">
         <v>6</v>
       </c>
@@ -1843,7 +1899,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A14" s="8"/>
       <c r="B14" s="4"/>
       <c r="C14" s="4" t="s">
@@ -1853,7 +1909,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="15" spans="1:8" ht="60" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:8" ht="43.2" x14ac:dyDescent="0.55000000000000004">
       <c r="A15" s="7" t="s">
         <v>16</v>
       </c>
@@ -1865,7 +1921,7 @@
       </c>
       <c r="H15" s="10"/>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="B16" s="5">
         <v>2</v>
       </c>
@@ -1873,7 +1929,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A17" s="8"/>
       <c r="B17" s="4"/>
       <c r="C17" s="4" t="s">
@@ -1883,7 +1939,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="18" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:7" ht="57.6" x14ac:dyDescent="0.55000000000000004">
       <c r="A18" s="7" t="s">
         <v>35</v>
       </c>
@@ -1894,7 +1950,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="B19" s="5">
         <v>2</v>
       </c>
@@ -1902,7 +1958,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="G21" s="10"/>
     </row>
   </sheetData>
@@ -1919,31 +1975,31 @@
       <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.83984375" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col min="1" max="1" width="15.140625" style="5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8.85546875" style="5"/>
-    <col min="3" max="4" width="43.85546875" style="5" bestFit="1" customWidth="1"/>
-    <col min="5" max="16384" width="8.85546875" style="1"/>
+    <col min="1" max="1" width="15.15625" style="5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.83984375" style="5"/>
+    <col min="3" max="4" width="43.83984375" style="5" bestFit="1" customWidth="1"/>
+    <col min="5" max="16384" width="8.83984375" style="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" s="4" t="s">
         <v>6</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" s="5" t="s">
         <v>0</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" s="5" t="s">
         <v>1</v>
       </c>
@@ -1951,12 +2007,12 @@
         <v>31</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" s="5" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="C7" s="5" t="s">
         <v>4</v>
       </c>
@@ -1964,7 +2020,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A8" s="5" t="s">
         <v>3</v>
       </c>
@@ -1972,10 +2028,10 @@
         <v>1</v>
       </c>
       <c r="C8" s="5" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="B9" s="5">
         <v>2</v>
       </c>
@@ -1983,34 +2039,34 @@
         <v>13</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="B10" s="5">
         <v>3</v>
       </c>
       <c r="C10" s="5" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A11" s="6"/>
       <c r="B11" s="5">
         <v>4</v>
       </c>
       <c r="D11" s="5" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A12" s="6"/>
       <c r="B12" s="5">
         <v>5</v>
       </c>
       <c r="D12" s="5" t="s">
-        <v>108</v>
+        <v>103</v>
       </c>
       <c r="H12" s="10"/>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A13" s="8"/>
       <c r="B13" s="4"/>
       <c r="C13" s="4" t="s">
@@ -2021,7 +2077,7 @@
       </c>
       <c r="H13" s="10"/>
     </row>
-    <row r="14" spans="1:8" ht="75" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:8" ht="72" x14ac:dyDescent="0.55000000000000004">
       <c r="A14" s="7" t="s">
         <v>25</v>
       </c>
@@ -2032,7 +2088,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A15" s="7"/>
       <c r="B15" s="5">
         <v>2</v>
@@ -2042,13 +2098,13 @@
       </c>
       <c r="G15" s="10"/>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A16" s="8"/>
       <c r="B16" s="4"/>
       <c r="C16" s="4"/>
       <c r="D16" s="4"/>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:1" x14ac:dyDescent="0.55000000000000004">
       <c r="A17" s="7"/>
     </row>
   </sheetData>
@@ -2061,20 +2117,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A3:L17"/>
   <sheetViews>
-    <sheetView topLeftCell="A2" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.83984375" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
     <col min="1" max="1" width="19" style="5" customWidth="1"/>
-    <col min="2" max="2" width="8.85546875" style="5"/>
-    <col min="3" max="3" width="36.140625" style="5" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="36.42578125" style="5" bestFit="1" customWidth="1"/>
-    <col min="5" max="16384" width="8.85546875" style="1"/>
+    <col min="2" max="2" width="8.83984375" style="5"/>
+    <col min="3" max="3" width="36.15625" style="5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="36.41796875" style="5" bestFit="1" customWidth="1"/>
+    <col min="5" max="16384" width="8.83984375" style="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" s="4" t="s">
         <v>6</v>
       </c>
@@ -2082,7 +2138,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" s="5" t="s">
         <v>0</v>
       </c>
@@ -2090,7 +2146,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" s="5" t="s">
         <v>1</v>
       </c>
@@ -2099,12 +2155,12 @@
       </c>
       <c r="D5" s="12"/>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" s="5" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A7" s="4"/>
       <c r="B7" s="4"/>
       <c r="C7" s="4" t="s">
@@ -2114,7 +2170,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A8" s="5" t="s">
         <v>3</v>
       </c>
@@ -2125,7 +2181,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="B9" s="5">
         <v>2</v>
       </c>
@@ -2133,7 +2189,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="B10" s="5">
         <v>3</v>
       </c>
@@ -2141,7 +2197,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="B11" s="5">
         <v>4</v>
       </c>
@@ -2149,7 +2205,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A12" s="6"/>
       <c r="B12" s="5">
         <v>5</v>
@@ -2158,7 +2214,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A13" s="8"/>
       <c r="B13" s="4"/>
       <c r="C13" s="4" t="s">
@@ -2168,7 +2224,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="14" spans="1:8" ht="75" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:8" ht="57.6" x14ac:dyDescent="0.55000000000000004">
       <c r="A14" s="7" t="s">
         <v>44</v>
       </c>
@@ -2180,7 +2236,7 @@
       </c>
       <c r="H14" s="11"/>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A15" s="7"/>
       <c r="B15" s="5">
         <v>2</v>
@@ -2189,7 +2245,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="17" spans="12:12" x14ac:dyDescent="0.25">
+    <row r="17" spans="12:12" x14ac:dyDescent="0.55000000000000004">
       <c r="L17" s="10"/>
     </row>
   </sheetData>
@@ -2202,20 +2258,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A3:L17"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.83984375" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
     <col min="1" max="1" width="19" style="5" customWidth="1"/>
-    <col min="2" max="2" width="8.85546875" style="5"/>
+    <col min="2" max="2" width="8.83984375" style="5"/>
     <col min="3" max="3" width="39" style="5" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="36.42578125" style="5" bestFit="1" customWidth="1"/>
-    <col min="5" max="16384" width="8.85546875" style="1"/>
+    <col min="4" max="4" width="36.41796875" style="5" bestFit="1" customWidth="1"/>
+    <col min="5" max="16384" width="8.83984375" style="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" s="4" t="s">
         <v>6</v>
       </c>
@@ -2223,7 +2279,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" s="5" t="s">
         <v>0</v>
       </c>
@@ -2231,7 +2287,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" s="5" t="s">
         <v>1</v>
       </c>
@@ -2239,12 +2295,12 @@
         <v>40</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" s="5" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A7" s="4"/>
       <c r="B7" s="4"/>
       <c r="C7" s="4" t="s">
@@ -2254,7 +2310,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A8" s="5" t="s">
         <v>3</v>
       </c>
@@ -2265,7 +2321,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="B9" s="5">
         <v>2</v>
       </c>
@@ -2273,7 +2329,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="B10" s="5">
         <v>3</v>
       </c>
@@ -2281,7 +2337,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="B11" s="5">
         <v>4</v>
       </c>
@@ -2289,7 +2345,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A12" s="6"/>
       <c r="B12" s="5">
         <v>5</v>
@@ -2298,7 +2354,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A13" s="8"/>
       <c r="B13" s="4"/>
       <c r="C13" s="4" t="s">
@@ -2308,7 +2364,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="14" spans="1:8" ht="75" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:8" ht="57.6" x14ac:dyDescent="0.55000000000000004">
       <c r="A14" s="7" t="s">
         <v>44</v>
       </c>
@@ -2321,7 +2377,7 @@
       <c r="F14" s="10"/>
       <c r="H14" s="11"/>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A15" s="7"/>
       <c r="B15" s="5">
         <v>2</v>
@@ -2330,7 +2386,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="17" spans="12:12" x14ac:dyDescent="0.25">
+    <row r="17" spans="12:12" x14ac:dyDescent="0.55000000000000004">
       <c r="L17" s="10"/>
     </row>
   </sheetData>
@@ -2343,20 +2399,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A3:D13"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="A8" sqref="A8:D11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.83984375" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col min="1" max="1" width="15.140625" style="5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8.85546875" style="5"/>
-    <col min="3" max="3" width="40.28515625" style="5" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="39.28515625" style="5" bestFit="1" customWidth="1"/>
-    <col min="5" max="16384" width="8.85546875" style="1"/>
+    <col min="1" max="1" width="15.15625" style="5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.83984375" style="5"/>
+    <col min="3" max="3" width="40.26171875" style="5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="39.26171875" style="5" bestFit="1" customWidth="1"/>
+    <col min="5" max="16384" width="8.83984375" style="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" s="4" t="s">
         <v>6</v>
       </c>
@@ -2364,7 +2420,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" s="5" t="s">
         <v>0</v>
       </c>
@@ -2372,7 +2428,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" s="5" t="s">
         <v>1</v>
       </c>
@@ -2380,12 +2436,12 @@
         <v>63</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" s="5" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="C7" s="4" t="s">
         <v>4</v>
       </c>
@@ -2393,40 +2449,47 @@
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A8" s="5" t="s">
         <v>3</v>
       </c>
       <c r="B8" s="5">
         <v>1</v>
       </c>
-      <c r="D8" s="5" t="s">
+      <c r="C8" s="5" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="B9" s="5">
+        <v>2</v>
+      </c>
+      <c r="D9" s="5" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B9" s="5">
-        <v>2</v>
-      </c>
-      <c r="C9" s="5" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="B10" s="5">
         <v>3</v>
       </c>
-      <c r="D10" s="5" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C10" s="5" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A11" s="6"/>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B11" s="5">
+        <v>4</v>
+      </c>
+      <c r="D11" s="5" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A12" s="6"/>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B12" s="9"/>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A13" s="7"/>
     </row>
   </sheetData>
@@ -2439,20 +2502,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A3:I13"/>
   <sheetViews>
-    <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="E17" sqref="E17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.83984375" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col min="1" max="1" width="15.140625" style="5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8.85546875" style="5"/>
-    <col min="3" max="3" width="40.28515625" style="5" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="43.28515625" style="5" bestFit="1" customWidth="1"/>
-    <col min="5" max="16384" width="8.85546875" style="1"/>
+    <col min="1" max="1" width="15.15625" style="5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.83984375" style="5"/>
+    <col min="3" max="3" width="40.26171875" style="5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="45.62890625" style="5" bestFit="1" customWidth="1"/>
+    <col min="5" max="16384" width="8.83984375" style="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" s="4" t="s">
         <v>6</v>
       </c>
@@ -2460,7 +2523,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" s="5" t="s">
         <v>0</v>
       </c>
@@ -2468,7 +2531,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" s="5" t="s">
         <v>1</v>
       </c>
@@ -2476,12 +2539,12 @@
         <v>63</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" s="5" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="C7" s="4" t="s">
         <v>4</v>
       </c>
@@ -2490,41 +2553,47 @@
       </c>
       <c r="E7" s="10"/>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A8" s="5" t="s">
         <v>3</v>
       </c>
       <c r="B8" s="5">
         <v>1</v>
       </c>
-      <c r="D8" s="5" t="s">
+      <c r="C8" s="5" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+      <c r="B9" s="5">
+        <v>2</v>
+      </c>
+      <c r="D9" s="5" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B9" s="5">
-        <v>2</v>
-      </c>
-      <c r="C9" s="5" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="B10" s="5">
         <v>3</v>
       </c>
-      <c r="D10" s="5" t="s">
-        <v>99</v>
+      <c r="C10" s="5" t="s">
+        <v>106</v>
       </c>
       <c r="I10" s="10"/>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A11" s="6"/>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B11" s="5">
+        <v>4</v>
+      </c>
+      <c r="D11" s="5" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A12" s="6"/>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A13" s="7"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
ADicionadas partes do GOmes e Reis
</commit_message>
<xml_diff>
--- a/Fase 2/F2-Descrição_use_cases.xlsx
+++ b/Fase 2/F2-Descrição_use_cases.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="450" windowWidth="23040" windowHeight="8808" tabRatio="856" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="450" windowWidth="23040" windowHeight="8808" tabRatio="856" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Regista Apartamento" sheetId="7" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="240" uniqueCount="113">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="239" uniqueCount="115">
   <si>
     <r>
       <t xml:space="preserve">  </t>
@@ -434,6 +434,12 @@
   </si>
   <si>
     <t>Indica que o morador foi adicionado</t>
+  </si>
+  <si>
+    <t>Senhorio Autenticado com Apartamento registado</t>
+  </si>
+  <si>
+    <t>Indica que a renda inserida é inválida</t>
   </si>
 </sst>
 </file>
@@ -1384,7 +1390,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A3:F34"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
@@ -1933,15 +1939,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A3:H17"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.83984375" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col min="1" max="1" width="15.15625" style="5" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="15.15625" style="5" customWidth="1"/>
     <col min="2" max="2" width="8.83984375" style="5"/>
-    <col min="3" max="4" width="43.83984375" style="5" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="43.83984375" style="5" customWidth="1"/>
     <col min="5" max="16384" width="8.83984375" style="1"/>
   </cols>
   <sheetData>
@@ -1966,7 +1972,7 @@
         <v>1</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>30</v>
+        <v>113</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.55000000000000004">
@@ -1990,7 +1996,7 @@
         <v>1</v>
       </c>
       <c r="C8" s="5" t="s">
-        <v>89</v>
+        <v>101</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.55000000000000004">
@@ -2002,11 +2008,12 @@
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A10" s="6"/>
       <c r="B10" s="5">
         <v>3</v>
       </c>
-      <c r="C10" s="5" t="s">
-        <v>101</v>
+      <c r="D10" s="5" t="s">
+        <v>103</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.55000000000000004">
@@ -2015,17 +2022,10 @@
         <v>4</v>
       </c>
       <c r="D11" s="5" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A12" s="6"/>
-      <c r="B12" s="5">
-        <v>5</v>
-      </c>
-      <c r="D12" s="5" t="s">
-        <v>102</v>
-      </c>
       <c r="H12" s="10"/>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.55000000000000004">
@@ -2047,7 +2047,7 @@
         <v>1</v>
       </c>
       <c r="D14" s="5" t="s">
-        <v>16</v>
+        <v>114</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.55000000000000004">

</xml_diff>

<commit_message>
Vpp e Excels atualizados
</commit_message>
<xml_diff>
--- a/Fase 2/F2-Descrição_use_cases.xlsx
+++ b/Fase 2/F2-Descrição_use_cases.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="450" windowWidth="23040" windowHeight="8808" tabRatio="856" firstSheet="4" activeTab="10"/>
+    <workbookView xWindow="0" yWindow="450" windowWidth="23040" windowHeight="8808" tabRatio="856" firstSheet="4" activeTab="8"/>
   </bookViews>
   <sheets>
     <sheet name="Adicionar Despesa Extraord." sheetId="9" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="238" uniqueCount="113">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="252" uniqueCount="122">
   <si>
     <r>
       <t xml:space="preserve">  </t>
@@ -392,10 +392,6 @@
     <t>Apresenta a lista das despesas do morador</t>
   </si>
   <si>
-    <t>Excepção 2               (passo 3)
-[dados do apartamento inválidos]</t>
-  </si>
-  <si>
     <t>Indica que quer ver despesas pagas</t>
   </si>
   <si>
@@ -403,9 +399,6 @@
   </si>
   <si>
     <t>É acrescentado um morador ao apartamento</t>
-  </si>
-  <si>
-    <t>Não existe um apartamento no sistema</t>
   </si>
   <si>
     <t>Indica que o morador foi adicionado</t>
@@ -434,6 +427,42 @@
   </si>
   <si>
     <t>Autenticar Utilizador</t>
+  </si>
+  <si>
+    <t>Verifica se existe um Senhorio no sistema</t>
+  </si>
+  <si>
+    <t>Não existe um senhorio nem um apartamento no sistema</t>
+  </si>
+  <si>
+    <t>Fornece dados do Senhorio</t>
+  </si>
+  <si>
+    <t>Valida dados do Senhorio</t>
+  </si>
+  <si>
+    <t>Regista Senhorio</t>
+  </si>
+  <si>
+    <t>Indica que o Senhorio foi registado</t>
+  </si>
+  <si>
+    <t>Excepção 1               (passo 1)
+[existe um Senhorio no sistema]</t>
+  </si>
+  <si>
+    <t>Indica que já existe um Senhorio no Sistema</t>
+  </si>
+  <si>
+    <t>Excepção 2               (passo 3)
+[dados do Senhorio inválidos]</t>
+  </si>
+  <si>
+    <t>Regressa a 6</t>
+  </si>
+  <si>
+    <t>Excepção 3               (passo 7)
+[dados do apartamento inválidos]</t>
   </si>
 </sst>
 </file>
@@ -1019,7 +1048,7 @@
         <v>1</v>
       </c>
       <c r="C8" s="29" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="D8" s="26"/>
       <c r="E8" s="26"/>
@@ -1099,14 +1128,14 @@
     </row>
     <row r="14" spans="1:8" ht="72" x14ac:dyDescent="0.55000000000000004">
       <c r="A14" s="31" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="B14" s="29">
         <v>1</v>
       </c>
       <c r="C14" s="26"/>
       <c r="D14" s="29" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="E14" s="26"/>
       <c r="F14" s="33"/>
@@ -1293,7 +1322,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A3:I13"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="I28" sqref="I28"/>
     </sheetView>
   </sheetViews>
@@ -1352,7 +1381,7 @@
         <v>1</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.55000000000000004">
@@ -1378,7 +1407,7 @@
         <v>4</v>
       </c>
       <c r="D11" s="4" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.55000000000000004">
@@ -1589,7 +1618,7 @@
         <v>1</v>
       </c>
       <c r="C8" s="19" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="D8" s="16"/>
       <c r="E8" s="16"/>
@@ -1669,14 +1698,14 @@
     </row>
     <row r="14" spans="1:8" ht="72" x14ac:dyDescent="0.55000000000000004">
       <c r="A14" s="21" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="B14" s="19">
         <v>1</v>
       </c>
       <c r="C14" s="16"/>
       <c r="D14" s="19" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="E14" s="16"/>
       <c r="F14" s="16"/>
@@ -1752,7 +1781,7 @@
         <v>2</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="7" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.55000000000000004">
@@ -1840,7 +1869,7 @@
         <v>9</v>
       </c>
       <c r="D16" s="4" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.55000000000000004">
@@ -2139,7 +2168,7 @@
         <v>1</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.55000000000000004">
@@ -2214,7 +2243,7 @@
         <v>1</v>
       </c>
       <c r="D14" s="4" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.55000000000000004">
@@ -2264,7 +2293,7 @@
         <v>6</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.55000000000000004">
@@ -2615,7 +2644,7 @@
         <v>3</v>
       </c>
       <c r="C10" s="12" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="D10" s="15"/>
       <c r="E10" s="11"/>
@@ -2737,7 +2766,7 @@
       </c>
       <c r="C17" s="11"/>
       <c r="D17" s="12" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
     </row>
   </sheetData>
@@ -2748,17 +2777,17 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A3:D16"/>
+  <dimension ref="A3:D28"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="G9" sqref="G9"/>
+    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="A28" sqref="A28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.83984375" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col min="1" max="1" width="15.15625" style="4" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="18.62890625" style="4" customWidth="1"/>
     <col min="2" max="2" width="8.83984375" style="4"/>
-    <col min="3" max="3" width="31.83984375" style="4" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="46.3125" style="4" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="32.68359375" style="4" customWidth="1"/>
     <col min="5" max="16384" width="8.83984375" style="1"/>
   </cols>
@@ -2784,7 +2813,7 @@
         <v>1</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>103</v>
+        <v>112</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.55000000000000004">
@@ -2807,65 +2836,164 @@
       <c r="B8" s="4">
         <v>1</v>
       </c>
-      <c r="C8" s="4" t="s">
-        <v>81</v>
+      <c r="D8" s="4" t="s">
+        <v>111</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="B9" s="4">
-        <f>B8+1</f>
-        <v>2</v>
-      </c>
-      <c r="D9" s="4" t="s">
+        <f>1+B8</f>
+        <v>2</v>
+      </c>
+      <c r="C9" s="4" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="B10" s="29">
+        <f t="shared" ref="B10:B16" si="0">1+B9</f>
+        <v>3</v>
+      </c>
+      <c r="D10" s="4" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="B11" s="29">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="D11" s="4" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="B12" s="29">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="D12" s="4" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="B13" s="29">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
+      <c r="C13" s="4" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="B14" s="29">
+        <f t="shared" si="0"/>
+        <v>7</v>
+      </c>
+      <c r="D14" s="4" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="B10" s="4">
-        <f t="shared" ref="B10:B11" si="0">B9+1</f>
-        <v>3</v>
-      </c>
-      <c r="D10" s="4" t="s">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="B15" s="29">
+        <f t="shared" si="0"/>
+        <v>8</v>
+      </c>
+      <c r="D15" s="4" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="B11" s="4">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="B16" s="29">
         <f t="shared" si="0"/>
-        <v>4</v>
-      </c>
-      <c r="D11" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="D16" s="4" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A14" s="7"/>
-      <c r="B14" s="3"/>
-      <c r="C14" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="D14" s="3" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" ht="72" x14ac:dyDescent="0.55000000000000004">
-      <c r="A15" s="6" t="s">
-        <v>99</v>
-      </c>
-      <c r="B15" s="4">
-        <v>1</v>
-      </c>
-      <c r="D15" s="10" t="s">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A17" s="32"/>
+      <c r="B17" s="28"/>
+      <c r="C17" s="28" t="s">
+        <v>4</v>
+      </c>
+      <c r="D17" s="28" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" ht="72" x14ac:dyDescent="0.55000000000000004">
+      <c r="A18" s="31" t="s">
+        <v>117</v>
+      </c>
+      <c r="B18" s="29">
+        <v>1</v>
+      </c>
+      <c r="C18" s="29"/>
+      <c r="D18" s="10" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A19" s="32"/>
+      <c r="B19" s="28"/>
+      <c r="C19" s="28" t="s">
+        <v>4</v>
+      </c>
+      <c r="D19" s="28" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" ht="72" x14ac:dyDescent="0.55000000000000004">
+      <c r="A20" s="31" t="s">
+        <v>119</v>
+      </c>
+      <c r="B20" s="29">
+        <v>1</v>
+      </c>
+      <c r="C20" s="29"/>
+      <c r="D20" s="10" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A16" s="6"/>
-      <c r="B16" s="4">
-        <v>2</v>
-      </c>
-      <c r="D16" s="4" t="s">
-        <v>17</v>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A21" s="31"/>
+      <c r="B21" s="29">
+        <v>2</v>
+      </c>
+      <c r="C21" s="29"/>
+      <c r="D21" s="29" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A26" s="7"/>
+      <c r="B26" s="3"/>
+      <c r="C26" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="D26" s="3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" ht="72" x14ac:dyDescent="0.55000000000000004">
+      <c r="A27" s="6" t="s">
+        <v>121</v>
+      </c>
+      <c r="B27" s="4">
+        <v>1</v>
+      </c>
+      <c r="D27" s="10" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A28" s="6"/>
+      <c r="B28" s="4">
+        <v>2</v>
+      </c>
+      <c r="D28" s="4" t="s">
+        <v>120</v>
       </c>
     </row>
   </sheetData>

</xml_diff>